<commit_message>
UI updates to the app
</commit_message>
<xml_diff>
--- a/inst/extdata/flow_template.xlsx
+++ b/inst/extdata/flow_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sccwrp.sharepoint.com/sites/Staff/Shared Documents/P Drive/Data/DuyNguyen/Projects/bmp-hydrology-calculator/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{F0F45A3E-2991-4552-98CD-6C047B03EB08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B8989D91-DB7C-4302-A686-398D8135DC75}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{F0F45A3E-2991-4552-98CD-6C047B03EB08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{736D61F0-D4F0-4B43-A91B-62662829BA01}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-45" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -186,45 +186,6 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>It is required that the column names and tab names in the templates remain unchanged.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1600">
-            <a:solidFill>
-              <a:schemeClr val="dk1"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1600">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>**Flow Analysis:**</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1600">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
             <a:t>Flow data should be copy-pasted from a user's datasheet to the downloaded data template. Up to four flows can be accommodated for analysis. The available flow types are inflow 1, inflow 2, outflow, and bypass. Refer to the Methods tab for an illustration of the possible flow type configurations. A user does not need to submit all four types; any combination of the flow types is acceptable. A user can only submit flow data for a single rain event. If any of the data types are not applicable, leave the tab blank (as is).</a:t>
           </a:r>
         </a:p>
@@ -289,7 +250,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>**Data Requirements**</a:t>
+            <a:t>**Data Requirements:**</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -359,11 +320,22 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>4. The column names and the tab names must not be changed from the template.</a:t>
+            <a:t>4. The inflow1 and outflow must have data.</a:t>
           </a:r>
-          <a:endParaRPr lang="en-US" sz="1600">
-            <a:effectLst/>
-          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>5. **The column names and the tab names must not be changed from the template**.</a:t>
+          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -758,29 +730,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="02ea596c-bf3f-4512-ad68-024a720c79b2">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="959569b2-1f16-4dd0-b5ed-bb064e5cd07e" xsi:nil="true"/>
-    <OldForms xmlns="02ea596c-bf3f-4512-ad68-024a720c79b2" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000C0FD75001275F4DBA43EB7BE58C8A34" ma:contentTypeVersion="21" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="75e20f4bf570a29fdd68b6ac0ce9f23e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="02ea596c-bf3f-4512-ad68-024a720c79b2" xmlns:ns3="959569b2-1f16-4dd0-b5ed-bb064e5cd07e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7d8333fcdd8157586878df4d15f204f2" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -1054,27 +1003,30 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="02ea596c-bf3f-4512-ad68-024a720c79b2">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="959569b2-1f16-4dd0-b5ed-bb064e5cd07e" xsi:nil="true"/>
+    <OldForms xmlns="02ea596c-bf3f-4512-ad68-024a720c79b2" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{30E79D0C-F610-4EAE-A025-AE59D3D7877F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC2A99C6-72A4-4F0E-BB64-9F38352613FB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="02ea596c-bf3f-4512-ad68-024a720c79b2"/>
-    <ds:schemaRef ds:uri="959569b2-1f16-4dd0-b5ed-bb064e5cd07e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2475D521-D46A-452A-8F4A-E4D7CE7B9C44}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1092,4 +1044,24 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC2A99C6-72A4-4F0E-BB64-9F38352613FB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="02ea596c-bf3f-4512-ad68-024a720c79b2"/>
+    <ds:schemaRef ds:uri="959569b2-1f16-4dd0-b5ed-bb064e5cd07e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{30E79D0C-F610-4EAE-A025-AE59D3D7877F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>